<commit_message>
Add functionality for adding groups to the db
</commit_message>
<xml_diff>
--- a/custom/excel_sheet.xlsx
+++ b/custom/excel_sheet.xlsx
@@ -437,22 +437,22 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="0" t="inlineStr">
         <is>
           <t>Basketball</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="0" t="inlineStr">
         <is>
           <t>group b, group a</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="0" t="inlineStr">
         <is>
           <t>2022-01-11</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="0" t="inlineStr">
         <is>
           <t>01:20:00</t>
         </is>
@@ -469,14 +469,55 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15" customHeight="1"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>okokokok</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>-615761128</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>okokokok</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>-615761128</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>okokokok</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>-615761128</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>annie's test</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-485430438</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add real groups functionality.
</commit_message>
<xml_diff>
--- a/custom/excel_sheet.xlsx
+++ b/custom/excel_sheet.xlsx
@@ -355,7 +355,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,28 @@
       <c r="D5" s="0" t="inlineStr">
         <is>
           <t>01:20:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Volleyball</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>okokokok</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2021-11-23</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>11:00:00</t>
         </is>
       </c>
     </row>
@@ -508,12 +530,12 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="0" t="inlineStr">
         <is>
           <t>annie's test</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="0" t="n">
         <v>-485430438</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add attendance sheet logic. Changes to handle response.
</commit_message>
<xml_diff>
--- a/custom/excel_sheet.xlsx
+++ b/custom/excel_sheet.xlsx
@@ -357,7 +357,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -368,6 +368,161 @@
     <col width="12.63" customWidth="1" style="4" min="1" max="6"/>
   </cols>
   <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>Basketball</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>annie's test, okokokok</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-11</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>23:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>Basketball</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>okokokok</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-11</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>23:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>Basketball</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>okokokok</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-11</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>23:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>Basketball</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>okokokok</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-11</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>23:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>Basketball</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>okokokok</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-11</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>23:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>Basketball</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>okokokok</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-11</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>23:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Basketball</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>okokokok:13</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2021-11-11</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1" s="4"/>
     <row r="14" ht="15.75" customHeight="1" s="4"/>
     <row r="15" ht="15.75" customHeight="1" s="4"/>
     <row r="16" ht="15.75" customHeight="1" s="4"/>
@@ -1347,7 +1502,6 @@
     <row r="990" ht="15.75" customHeight="1" s="4"/>
     <row r="991" ht="15.75" customHeight="1" s="4"/>
     <row r="992" ht="15.75" customHeight="1" s="4"/>
-    <row r="993" ht="15.75" customHeight="1" s="4"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>